<commit_message>
Revert "Merge branch 'wangtao'"
This reverts commit b76eca0e60b58b8d1667764632d6601768049e12.
</commit_message>
<xml_diff>
--- a/学员信息统计.xlsx
+++ b/学员信息统计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9552"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -280,7 +280,7 @@
     <t>https://github.com/wangtap/JaveS</t>
   </si>
   <si>
-    <t>https://github.com/wangtap/JaveS/tree/master/Project</t>
+    <t>https://github.com/wangtap/JaveS/tree/master/Syster</t>
   </si>
   <si>
     <t>https://github.com/wangtap/JaveS/tree/master/HomeWork</t>
@@ -361,9 +361,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -406,7 +406,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -420,31 +472,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,31 +511,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -497,49 +534,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -562,19 +562,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,163 +742,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,11 +841,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -876,6 +891,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -887,6 +911,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -905,39 +938,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -946,10 +946,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -958,16 +958,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -976,115 +976,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1250,6 +1250,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1505,27 +1510,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:F28"/>
+      <selection activeCell="G22" sqref="G22:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="49.1296296296296" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.1333333333333" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="49.1296296296296" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.1333333333333" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="49.1296296296296" style="1" customWidth="1"/>
+    <col min="8" max="8" width="49.1333333333333" style="1" customWidth="1"/>
     <col min="9" max="10" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2529,7 +2533,7 @@
     <hyperlink ref="G9" r:id="rId28" display="https://github.com/DmeoL/LXHomeWork"/>
     <hyperlink ref="G17" r:id="rId66" display="https://github.com/Larry21gram/mysql_homework"/>
     <hyperlink ref="G15" r:id="rId67" display="https://github.com/xuhan961228/xuhan2/blob/master/1222html%E7%AC%94%E8%AE%B0.txt"/>
-    <hyperlink ref="E28" r:id="rId68" display="https://github.com/wangtap/JaveS/tree/master/Project" tooltip="https://github.com/wangtap/JaveS/tree/master/Project"/>
+    <hyperlink ref="E28" r:id="rId68" display="https://github.com/wangtap/JaveS/tree/master/Syster" tooltip="https://github.com/wangtap/JaveS/tree/master/Syster"/>
     <hyperlink ref="G6" r:id="rId69" display="https://github.com/NotTwoChen/Java-StudyData/tree/master/%E4%BD%9C%E4%B8%9A%E9%9B%86"/>
     <hyperlink ref="G8" r:id="rId70" display="https://github.com/FineDreams/JavaStudy/tree/master/%E4%BD%9C%E4%B8%9A"/>
     <hyperlink ref="E34" r:id="rId71" display="https://github.com/chenhonggangNZ/quitWorkSpace"/>

</xml_diff>